<commit_message>
Plot with quality comparison fixed.
</commit_message>
<xml_diff>
--- a/doc/ammm_project_experiments.xlsx
+++ b/doc/ammm_project_experiments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7090" tabRatio="487" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7090" tabRatio="487"/>
   </bookViews>
   <sheets>
     <sheet name="ILP" sheetId="1" r:id="rId1"/>
@@ -462,9 +462,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>ILP!$B$1:$D$1</c:f>
+              <c:f>ILP!$B$1:$E$1</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>instance_30_1484859967.dat</c:v>
                 </c:pt>
@@ -473,16 +473,19 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>instance_40_1484854749.dat</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>intance_100_1484842984.dat</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ILP!$B$15:$D$15</c:f>
+              <c:f>ILP!$B$15:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.94738794289487327</c:v>
                 </c:pt>
@@ -491,6 +494,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.9259385563167114</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.86302766235909767</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -534,12 +540,32 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>ILP!$B$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>instance_30_1484859967.dat</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>instance_50_1484852111.dat</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>instance_40_1484854749.dat</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>intance_100_1484842984.dat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ILP!$B$16:$D$16</c:f>
+              <c:f>ILP!$B$16:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.90003523757875348</c:v>
                 </c:pt>
@@ -548,6 +574,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.96154878421100798</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.87501296746225898</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -591,12 +620,32 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>ILP!$B$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>instance_30_1484859967.dat</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>instance_50_1484852111.dat</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>instance_40_1484854749.dat</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>intance_100_1484842984.dat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ILP!$B$17:$D$17</c:f>
+              <c:f>ILP!$B$17:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -605,6 +654,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.96154878421100798</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.87501248139248322</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -648,12 +700,32 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>ILP!$B$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>instance_30_1484859967.dat</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>instance_50_1484852111.dat</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>instance_40_1484854749.dat</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>intance_100_1484842984.dat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ILP!$B$18:$D$18</c:f>
+              <c:f>ILP!$B$18:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.94738794289487327</c:v>
                 </c:pt>
@@ -662,6 +734,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.9999916024151454</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.92647890699727897</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5919,10 +5994,10 @@
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>425450</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5950,15 +6025,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>863600</xdr:colOff>
+      <xdr:colOff>876300</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5986,15 +6061,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>869950</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:colOff>889000</xdr:colOff>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6407,8 +6482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R50" sqref="R50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6600,7 +6675,7 @@
         <v>2500719</v>
       </c>
       <c r="E12">
-        <v>7000715</v>
+        <v>6800715</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -6701,7 +6776,7 @@
       </c>
       <c r="E18">
         <f>$E$8/E12</f>
-        <v>0.90001078461271455</v>
+        <v>0.92647890699727897</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -7673,7 +7748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>